<commit_message>
Change EBase.py to read from overal spreadsheet Added metadata sheet in cytation_H1_place
</commit_message>
<xml_diff>
--- a/cytation_H1_plate1.xlsx
+++ b/cytation_H1_plate1.xlsx
@@ -1,13 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\School Stuff\Sem 7\FYP\EBase + PBase\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D25F620-D0D5-4A25-AE54-FE04AC23DCA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="9435" windowHeight="6915"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Plate 1 - Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Metadata" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="MethodPointer">13461632</definedName>
@@ -17,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="280">
   <si>
     <t>Software Version</t>
   </si>
@@ -822,12 +829,48 @@
   <si>
     <t>Lagtime [RFP:535,600]</t>
   </si>
+  <si>
+    <t>Experiment ID</t>
+  </si>
+  <si>
+    <t>Measurement</t>
+  </si>
+  <si>
+    <t>Type of experiment</t>
+  </si>
+  <si>
+    <t>Temperature</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Plasmid name</t>
+  </si>
+  <si>
+    <t>ED1</t>
+  </si>
+  <si>
+    <t>OD600</t>
+  </si>
+  <si>
+    <t>Type1</t>
+  </si>
+  <si>
+    <t>Media1</t>
+  </si>
+  <si>
+    <t>plasmid1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -857,6 +900,14 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -943,7 +994,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -996,6 +1047,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1005,6 +1057,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1053,7 +1108,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1086,9 +1141,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1121,6 +1193,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1296,20 +1385,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:CU269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B173" sqref="B173"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="L72" sqref="L72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1317,7 +1406,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" ht="66" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -1325,7 +1414,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1333,7 +1422,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1341,7 +1430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -1349,7 +1438,7 @@
         <v>43888</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1357,7 +1446,7 @@
         <v>0.73694444444444451</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -1365,7 +1454,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -1373,7 +1462,7 @@
         <v>269921</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
@@ -1381,13 +1470,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1"/>
     </row>
-    <row r="14" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -1395,7 +1484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1403,7 +1492,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>20</v>
       </c>
@@ -1411,19 +1500,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B18" s="1"/>
     </row>
-    <row r="19" spans="1:2" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -1431,7 +1520,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>26</v>
       </c>
@@ -1439,13 +1528,13 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>29</v>
       </c>
@@ -1453,31 +1542,31 @@
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>29</v>
       </c>
@@ -1485,55 +1574,55 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>29</v>
       </c>
@@ -1541,73 +1630,73 @@
         <v>43</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" ht="39.6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="51" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" ht="52.8" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="89.25" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" ht="92.4" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B45" s="1"/>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B46" s="1"/>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
         <v>47</v>
       </c>
       <c r="B48" s="1"/>
     </row>
-    <row r="50" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="6">
         <v>1</v>
@@ -1646,7 +1735,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B51" s="6" t="s">
         <v>48</v>
       </c>
@@ -1690,7 +1779,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B52" s="6" t="s">
         <v>62</v>
       </c>
@@ -1734,7 +1823,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
         <v>75</v>
       </c>
@@ -1778,7 +1867,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B54" s="6" t="s">
         <v>88</v>
       </c>
@@ -1822,7 +1911,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B55" s="6" t="s">
         <v>101</v>
       </c>
@@ -1866,7 +1955,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B56" s="6" t="s">
         <v>114</v>
       </c>
@@ -1910,7 +1999,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
         <v>127</v>
       </c>
@@ -1954,7 +2043,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B58" s="6" t="s">
         <v>140</v>
       </c>
@@ -1998,13 +2087,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
         <v>153</v>
       </c>
       <c r="B60" s="1"/>
     </row>
-    <row r="62" spans="1:99" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:99" ht="26.4" x14ac:dyDescent="0.25">
       <c r="B62" s="6" t="s">
         <v>9</v>
       </c>
@@ -2300,7 +2389,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="63" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B63" s="9">
         <v>8.6689814814814806E-3</v>
       </c>
@@ -2596,7 +2685,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B64" s="9">
         <v>1.9085648148148147E-2</v>
       </c>
@@ -2892,7 +2981,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="65" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B65" s="9">
         <v>2.9502314814814815E-2</v>
       </c>
@@ -3188,7 +3277,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="66" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B66" s="9">
         <v>3.9918981481481479E-2</v>
       </c>
@@ -3484,7 +3573,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="67" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B67" s="9">
         <v>5.033564814814815E-2</v>
       </c>
@@ -3780,7 +3869,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
     </row>
-    <row r="68" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B68" s="9">
         <v>6.0752314814814821E-2</v>
       </c>
@@ -4076,7 +4165,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="69" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B69" s="9">
         <v>7.1168981481481486E-2</v>
       </c>
@@ -4372,7 +4461,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="70" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B70" s="9">
         <v>8.1585648148148157E-2</v>
       </c>
@@ -4668,7 +4757,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="71" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B71" s="9">
         <v>9.2002314814814815E-2</v>
       </c>
@@ -4964,7 +5053,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="72" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B72" s="9">
         <v>0.10241898148148149</v>
       </c>
@@ -5260,7 +5349,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="73" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B73" s="9">
         <v>0.11283564814814816</v>
       </c>
@@ -5556,7 +5645,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="74" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B74" s="9">
         <v>0.12325231481481481</v>
       </c>
@@ -5852,7 +5941,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="75" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B75" s="9">
         <v>0.13366898148148149</v>
       </c>
@@ -6148,7 +6237,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="76" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B76" s="9">
         <v>0.14408564814814814</v>
       </c>
@@ -6444,7 +6533,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="77" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B77" s="9">
         <v>0.15450231481481483</v>
       </c>
@@ -6740,7 +6829,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="78" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B78" s="9">
         <v>0.16491898148148149</v>
       </c>
@@ -7036,7 +7125,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="79" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B79" s="9">
         <v>0.17533564814814814</v>
       </c>
@@ -7332,7 +7421,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="80" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B80" s="9">
         <v>0.1857523148148148</v>
       </c>
@@ -7628,7 +7717,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="81" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B81" s="9">
         <v>0.19616898148148146</v>
       </c>
@@ -7924,7 +8013,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="82" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B82" s="9">
         <v>0.20658564814814814</v>
       </c>
@@ -8220,7 +8309,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="83" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B83" s="9">
         <v>0.2170023148148148</v>
       </c>
@@ -8516,7 +8605,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="84" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B84" s="9">
         <v>0.22741898148148146</v>
       </c>
@@ -8812,7 +8901,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="85" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B85" s="9">
         <v>0.23783564814814814</v>
       </c>
@@ -9108,7 +9197,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="86" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B86" s="9">
         <v>0.2482523148148148</v>
       </c>
@@ -9404,7 +9493,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="87" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B87" s="9">
         <v>0.25866898148148149</v>
       </c>
@@ -9700,7 +9789,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="88" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B88" s="9">
         <v>0.26908564814814812</v>
       </c>
@@ -9996,7 +10085,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="89" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B89" s="9">
         <v>0.2795023148148148</v>
       </c>
@@ -10292,7 +10381,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="90" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B90" s="9">
         <v>0.28991898148148149</v>
       </c>
@@ -10588,7 +10677,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="91" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B91" s="9">
         <v>0.30033564814814812</v>
       </c>
@@ -10884,7 +10973,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="92" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B92" s="9">
         <v>0.3107523148148148</v>
       </c>
@@ -11180,7 +11269,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="93" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B93" s="9">
         <v>0.32116898148148149</v>
       </c>
@@ -11476,7 +11565,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="94" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B94" s="9">
         <v>0.33158564814814812</v>
       </c>
@@ -11772,7 +11861,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="95" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B95" s="9">
         <v>0.3420023148148148</v>
       </c>
@@ -12068,13 +12157,13 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="97" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
         <v>251</v>
       </c>
       <c r="B97" s="1"/>
     </row>
-    <row r="99" spans="1:99" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:99" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B99" s="6" t="s">
         <v>9</v>
       </c>
@@ -12370,7 +12459,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="100" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B100" s="9">
         <v>9.2476851851851852E-3</v>
       </c>
@@ -12666,7 +12755,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="101" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B101" s="9">
         <v>1.9664351851851853E-2</v>
       </c>
@@ -12962,7 +13051,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="102" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B102" s="9">
         <v>3.0081018518518521E-2</v>
       </c>
@@ -13258,7 +13347,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="103" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B103" s="9">
         <v>4.0497685185185185E-2</v>
       </c>
@@ -13554,7 +13643,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="104" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B104" s="9">
         <v>5.0914351851851856E-2</v>
       </c>
@@ -13850,7 +13939,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="105" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B105" s="9">
         <v>6.1331018518518521E-2</v>
       </c>
@@ -14146,7 +14235,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="106" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B106" s="9">
         <v>7.1747685185185192E-2</v>
       </c>
@@ -14442,7 +14531,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="107" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B107" s="9">
         <v>8.216435185185185E-2</v>
       </c>
@@ -14738,7 +14827,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="108" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B108" s="9">
         <v>9.2581018518518521E-2</v>
       </c>
@@ -15034,7 +15123,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="109" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B109" s="9">
         <v>0.10299768518518519</v>
       </c>
@@ -15330,7 +15419,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="110" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B110" s="9">
         <v>0.11341435185185185</v>
       </c>
@@ -15626,7 +15715,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="111" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B111" s="9">
         <v>0.12383101851851852</v>
       </c>
@@ -15922,7 +16011,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B112" s="9">
         <v>0.13424768518518518</v>
       </c>
@@ -16218,7 +16307,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="113" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B113" s="9">
         <v>0.14466435185185186</v>
       </c>
@@ -16514,7 +16603,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="114" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B114" s="9">
         <v>0.15508101851851852</v>
       </c>
@@ -16810,7 +16899,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="115" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B115" s="9">
         <v>0.16549768518518518</v>
       </c>
@@ -17106,7 +17195,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="116" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B116" s="9">
         <v>0.17591435185185186</v>
       </c>
@@ -17402,7 +17491,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="117" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B117" s="9">
         <v>0.18633101851851852</v>
       </c>
@@ -17698,7 +17787,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="118" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B118" s="9">
         <v>0.19674768518518518</v>
       </c>
@@ -17994,7 +18083,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="119" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B119" s="9">
         <v>0.20716435185185186</v>
       </c>
@@ -18290,7 +18379,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="120" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B120" s="9">
         <v>0.21758101851851852</v>
       </c>
@@ -18586,7 +18675,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="121" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B121" s="9">
         <v>0.22799768518518518</v>
       </c>
@@ -18882,7 +18971,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="122" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B122" s="9">
         <v>0.23841435185185186</v>
       </c>
@@ -19178,7 +19267,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="123" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B123" s="9">
         <v>0.24883101851851852</v>
       </c>
@@ -19474,7 +19563,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="124" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B124" s="9">
         <v>0.25924768518518521</v>
       </c>
@@ -19770,7 +19859,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="125" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B125" s="9">
         <v>0.26966435185185184</v>
       </c>
@@ -20066,7 +20155,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="126" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B126" s="9">
         <v>0.28008101851851852</v>
       </c>
@@ -20362,7 +20451,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="127" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B127" s="9">
         <v>0.29049768518518521</v>
       </c>
@@ -20658,7 +20747,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="128" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B128" s="9">
         <v>0.30091435185185184</v>
       </c>
@@ -20954,7 +21043,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="129" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B129" s="9">
         <v>0.31133101851851852</v>
       </c>
@@ -21250,7 +21339,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="130" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B130" s="9">
         <v>0.32174768518518521</v>
       </c>
@@ -21546,7 +21635,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="131" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B131" s="9">
         <v>0.33216435185185184</v>
       </c>
@@ -21842,7 +21931,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="132" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B132" s="9">
         <v>0.34258101851851852</v>
       </c>
@@ -22138,13 +22227,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="134" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A134" s="4" t="s">
         <v>253</v>
       </c>
       <c r="B134" s="1"/>
     </row>
-    <row r="136" spans="1:99" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:99" ht="39.6" x14ac:dyDescent="0.25">
       <c r="B136" s="6" t="s">
         <v>9</v>
       </c>
@@ -22440,7 +22529,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="137" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B137" s="9">
         <v>9.8263888888888897E-3</v>
       </c>
@@ -22736,7 +22825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="138" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B138" s="9">
         <v>2.0243055555555552E-2</v>
       </c>
@@ -23032,7 +23121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B139" s="9">
         <v>3.0659722222222224E-2</v>
       </c>
@@ -23328,7 +23417,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="140" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B140" s="9">
         <v>4.1076388888888891E-2</v>
       </c>
@@ -23624,7 +23713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B141" s="9">
         <v>5.1493055555555556E-2</v>
       </c>
@@ -23920,7 +24009,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="142" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B142" s="9">
         <v>6.190972222222222E-2</v>
       </c>
@@ -24216,7 +24305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B143" s="9">
         <v>7.2326388888888885E-2</v>
       </c>
@@ -24512,7 +24601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="144" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B144" s="9">
         <v>8.2743055555555556E-2</v>
       </c>
@@ -24808,7 +24897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B145" s="9">
         <v>9.3159722222222227E-2</v>
       </c>
@@ -25104,7 +25193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="146" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B146" s="9">
         <v>0.10357638888888888</v>
       </c>
@@ -25400,7 +25489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="147" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B147" s="9">
         <v>0.11399305555555556</v>
       </c>
@@ -25696,7 +25785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="148" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B148" s="9">
         <v>0.12440972222222223</v>
       </c>
@@ -25992,7 +26081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="149" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B149" s="9">
         <v>0.1348263888888889</v>
       </c>
@@ -26288,7 +26377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B150" s="9">
         <v>0.14524305555555556</v>
       </c>
@@ -26584,7 +26673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="151" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B151" s="9">
         <v>0.15565972222222221</v>
       </c>
@@ -26880,7 +26969,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="152" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B152" s="9">
         <v>0.1660763888888889</v>
       </c>
@@ -27176,7 +27265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="153" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B153" s="9">
         <v>0.17649305555555558</v>
       </c>
@@ -27472,7 +27561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B154" s="9">
         <v>0.18690972222222221</v>
       </c>
@@ -27768,7 +27857,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B155" s="9">
         <v>0.1973263888888889</v>
       </c>
@@ -28064,7 +28153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="156" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B156" s="9">
         <v>0.20774305555555558</v>
       </c>
@@ -28360,7 +28449,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B157" s="9">
         <v>0.21815972222222224</v>
       </c>
@@ -28656,7 +28745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B158" s="9">
         <v>0.22857638888888887</v>
       </c>
@@ -28952,7 +29041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="159" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B159" s="9">
         <v>0.23899305555555558</v>
       </c>
@@ -29248,7 +29337,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="160" spans="2:99" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:99" x14ac:dyDescent="0.25">
       <c r="B160" s="9">
         <v>0.24940972222222224</v>
       </c>
@@ -29544,7 +29633,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="161" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B161" s="9">
         <v>0.25982638888888893</v>
       </c>
@@ -29840,7 +29929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="162" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B162" s="9">
         <v>0.27024305555555556</v>
       </c>
@@ -30136,7 +30225,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="163" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B163" s="9">
         <v>0.28065972222222224</v>
       </c>
@@ -30432,7 +30521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B164" s="9">
         <v>0.29107638888888893</v>
       </c>
@@ -30728,7 +30817,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="165" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B165" s="9">
         <v>0.30149305555555556</v>
       </c>
@@ -31024,7 +31113,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B166" s="9">
         <v>0.31190972222222219</v>
       </c>
@@ -31320,7 +31409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B167" s="9">
         <v>0.32232638888888893</v>
       </c>
@@ -31616,7 +31705,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="168" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B168" s="9">
         <v>0.33274305555555556</v>
       </c>
@@ -31912,7 +32001,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="169" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B169" s="9">
         <v>0.34315972222222224</v>
       </c>
@@ -32208,13 +32297,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="171" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:99" x14ac:dyDescent="0.25">
       <c r="A171" s="4" t="s">
         <v>255</v>
       </c>
       <c r="B171" s="1"/>
     </row>
-    <row r="173" spans="1:99" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:99" x14ac:dyDescent="0.25">
       <c r="B173" s="5"/>
       <c r="C173" s="6">
         <v>1</v>
@@ -32253,7 +32342,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="174" spans="1:99" ht="18" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:99" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B174" s="15" t="s">
         <v>48</v>
       </c>
@@ -32297,7 +32386,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="175" spans="1:99" ht="18" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:99" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B175" s="16"/>
       <c r="C175" s="12">
         <v>1</v>
@@ -32339,7 +32428,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="176" spans="1:99" ht="18" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:99" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B176" s="16"/>
       <c r="C176" s="13">
         <v>0.13887731481481483</v>
@@ -32381,7 +32470,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="177" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B177" s="16"/>
       <c r="C177" s="13">
         <v>8.5000000000000006E-2</v>
@@ -32423,7 +32512,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="178" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B178" s="16"/>
       <c r="C178" s="12">
         <v>-14733.333000000001</v>
@@ -32465,7 +32554,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="179" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B179" s="16"/>
       <c r="C179" s="12">
         <v>1</v>
@@ -32507,7 +32596,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="180" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B180" s="16"/>
       <c r="C180" s="13">
         <v>1.4456018518518519E-2</v>
@@ -32549,7 +32638,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="181" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B181" s="16"/>
       <c r="C181" s="13">
         <v>9.2476851851851852E-3</v>
@@ -32591,7 +32680,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="182" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B182" s="16"/>
       <c r="C182" s="12">
         <v>-866.66700000000003</v>
@@ -32633,7 +32722,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="183" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B183" s="16"/>
       <c r="C183" s="12">
         <v>1</v>
@@ -32675,7 +32764,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="184" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B184" s="16"/>
       <c r="C184" s="13">
         <v>0.16086805555555556</v>
@@ -32717,7 +32806,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="185" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B185" s="17"/>
       <c r="C185" s="14">
         <v>0.17008101851851853</v>
@@ -32759,7 +32848,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="186" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B186" s="15" t="s">
         <v>62</v>
       </c>
@@ -32803,7 +32892,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="187" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B187" s="16"/>
       <c r="C187" s="12">
         <v>1</v>
@@ -32845,7 +32934,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="188" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B188" s="16"/>
       <c r="C188" s="13">
         <v>0.14929398148148149</v>
@@ -32887,7 +32976,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="189" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B189" s="16"/>
       <c r="C189" s="13">
         <v>9.5474537037037052E-2</v>
@@ -32929,7 +33018,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="190" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B190" s="16"/>
       <c r="C190" s="12">
         <v>-17933.332999999999</v>
@@ -32971,7 +33060,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="191" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B191" s="16"/>
       <c r="C191" s="12">
         <v>1</v>
@@ -33013,7 +33102,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="192" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B192" s="16"/>
       <c r="C192" s="13">
         <v>1.4456018518518519E-2</v>
@@ -33055,7 +33144,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="193" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B193" s="16"/>
       <c r="C193" s="13">
         <v>9.2476851851851852E-3</v>
@@ -33097,7 +33186,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="194" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B194" s="16"/>
       <c r="C194" s="12">
         <v>-866.66700000000003</v>
@@ -33139,7 +33228,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="195" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B195" s="16"/>
       <c r="C195" s="12">
         <v>1</v>
@@ -33181,7 +33270,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="196" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B196" s="16"/>
       <c r="C196" s="13">
         <v>0.20253472222222224</v>
@@ -33223,7 +33312,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="197" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B197" s="17"/>
       <c r="C197" s="14">
         <v>0.21015046296296294</v>
@@ -33265,7 +33354,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="198" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B198" s="15" t="s">
         <v>75</v>
       </c>
@@ -33309,7 +33398,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="199" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B199" s="16"/>
       <c r="C199" s="12">
         <v>1</v>
@@ -33351,7 +33440,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="200" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B200" s="16"/>
       <c r="C200" s="13">
         <v>0.13887731481481483</v>
@@ -33393,7 +33482,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="201" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B201" s="16"/>
       <c r="C201" s="13">
         <v>8.4710648148148146E-2</v>
@@ -33435,7 +33524,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="202" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B202" s="16"/>
       <c r="C202" s="12">
         <v>-12866.666999999999</v>
@@ -33477,7 +33566,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="203" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B203" s="16"/>
       <c r="C203" s="12">
         <v>1</v>
@@ -33519,7 +33608,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="204" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B204" s="16"/>
       <c r="C204" s="13">
         <v>1.4456018518518519E-2</v>
@@ -33561,7 +33650,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="205" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B205" s="16"/>
       <c r="C205" s="13">
         <v>9.2476851851851852E-3</v>
@@ -33603,7 +33692,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="206" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B206" s="16"/>
       <c r="C206" s="12">
         <v>800</v>
@@ -33645,7 +33734,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="207" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B207" s="16"/>
       <c r="C207" s="12">
         <v>1</v>
@@ -33687,7 +33776,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="208" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B208" s="16"/>
       <c r="C208" s="13">
         <v>1.503472222222222E-2</v>
@@ -33729,7 +33818,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="209" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B209" s="17"/>
       <c r="C209" s="14">
         <v>9.8263888888888897E-3</v>
@@ -33771,7 +33860,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="210" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B210" s="15" t="s">
         <v>88</v>
       </c>
@@ -33815,7 +33904,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="211" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B211" s="16"/>
       <c r="C211" s="12">
         <v>1</v>
@@ -33857,7 +33946,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="212" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B212" s="16"/>
       <c r="C212" s="13">
         <v>0.28471064814814812</v>
@@ -33899,7 +33988,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="213" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B213" s="16"/>
       <c r="C213" s="13">
         <v>0.13387731481481482</v>
@@ -33941,7 +34030,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="214" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B214" s="16"/>
       <c r="C214" s="12">
         <v>14266.666999999999</v>
@@ -33983,7 +34072,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="215" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B215" s="16"/>
       <c r="C215" s="12">
         <v>1</v>
@@ -34025,7 +34114,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="216" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B216" s="16"/>
       <c r="C216" s="13">
         <v>5.6122685185185185E-2</v>
@@ -34067,7 +34156,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="217" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B217" s="16"/>
       <c r="C217" s="13">
         <v>3.3101851851851848E-2</v>
@@ -34109,7 +34198,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="218" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B218" s="16"/>
       <c r="C218" s="12">
         <v>933.33299999999997</v>
@@ -34151,7 +34240,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="219" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B219" s="16"/>
       <c r="C219" s="12">
         <v>1</v>
@@ -34193,7 +34282,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="220" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B220" s="16"/>
       <c r="C220" s="13">
         <v>2.5451388888888888E-2</v>
@@ -34235,7 +34324,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="221" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B221" s="17"/>
       <c r="C221" s="14">
         <v>2.5451388888888888E-2</v>
@@ -34277,7 +34366,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="222" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B222" s="15" t="s">
         <v>101</v>
       </c>
@@ -34321,7 +34410,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="223" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B223" s="16"/>
       <c r="C223" s="12">
         <v>1</v>
@@ -34363,7 +34452,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="224" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B224" s="16"/>
       <c r="C224" s="13">
         <v>0.28471064814814812</v>
@@ -34405,7 +34494,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="225" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B225" s="16"/>
       <c r="C225" s="13">
         <v>0.17849537037037036</v>
@@ -34447,7 +34536,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="226" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B226" s="16"/>
       <c r="C226" s="12">
         <v>12533.333000000001</v>
@@ -34489,7 +34578,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="227" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B227" s="16"/>
       <c r="C227" s="12">
         <v>1</v>
@@ -34531,7 +34620,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="228" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B228" s="16"/>
       <c r="C228" s="13">
         <v>7.6956018518518521E-2</v>
@@ -34573,7 +34662,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="229" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B229" s="16"/>
       <c r="C229" s="13">
         <v>3.0914351851851849E-2</v>
@@ -34615,7 +34704,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="230" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B230" s="16"/>
       <c r="C230" s="12">
         <v>933.33299999999997</v>
@@ -34657,7 +34746,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="231" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B231" s="16"/>
       <c r="C231" s="12">
         <v>1</v>
@@ -34699,7 +34788,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="232" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B232" s="16"/>
       <c r="C232" s="13">
         <v>0.26503472222222219</v>
@@ -34741,7 +34830,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="233" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B233" s="17"/>
       <c r="C233" s="14">
         <v>0.27395833333333336</v>
@@ -34783,7 +34872,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="234" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B234" s="15" t="s">
         <v>114</v>
       </c>
@@ -34827,7 +34916,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="235" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B235" s="16"/>
       <c r="C235" s="12">
         <v>1</v>
@@ -34869,7 +34958,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="236" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B236" s="16"/>
       <c r="C236" s="13">
         <v>0.27429398148148149</v>
@@ -34911,7 +35000,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="237" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B237" s="16"/>
       <c r="C237" s="13">
         <v>0.19565972222222219</v>
@@ -34953,7 +35042,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="238" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B238" s="16"/>
       <c r="C238" s="12">
         <v>12000</v>
@@ -34995,7 +35084,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="239" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B239" s="16"/>
       <c r="C239" s="12">
         <v>1</v>
@@ -35037,7 +35126,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="240" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B240" s="16"/>
       <c r="C240" s="13">
         <v>5.6122685185185185E-2</v>
@@ -35079,7 +35168,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="241" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B241" s="16"/>
       <c r="C241" s="13">
         <v>2.8518518518518523E-2</v>
@@ -35121,7 +35210,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="242" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B242" s="16"/>
       <c r="C242" s="12">
         <v>1200</v>
@@ -35163,7 +35252,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="243" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B243" s="16"/>
       <c r="C243" s="12">
         <v>1</v>
@@ -35205,7 +35294,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="244" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B244" s="16"/>
       <c r="C244" s="13">
         <v>0.30670138888888887</v>
@@ -35247,7 +35336,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="245" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B245" s="17"/>
       <c r="C245" s="14">
         <v>0.30438657407407405</v>
@@ -35289,7 +35378,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="246" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B246" s="15" t="s">
         <v>127</v>
       </c>
@@ -35333,7 +35422,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="247" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B247" s="16"/>
       <c r="C247" s="12">
         <v>1</v>
@@ -35375,7 +35464,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="248" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B248" s="16"/>
       <c r="C248" s="13">
         <v>0.27429398148148149</v>
@@ -35417,7 +35506,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="249" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B249" s="16"/>
       <c r="C249" s="13">
         <v>0.28471064814814812</v>
@@ -35459,7 +35548,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="250" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B250" s="16"/>
       <c r="C250" s="12">
         <v>-600</v>
@@ -35501,7 +35590,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="251" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B251" s="16"/>
       <c r="C251" s="12">
         <v>1</v>
@@ -35543,7 +35632,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="252" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B252" s="16"/>
       <c r="C252" s="13">
         <v>8.7372685185185192E-2</v>
@@ -35585,7 +35674,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="253" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B253" s="16"/>
       <c r="C253" s="13">
         <v>8.9108796296296297E-2</v>
@@ -35627,7 +35716,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="254" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B254" s="16"/>
       <c r="C254" s="12">
         <v>1000</v>
@@ -35669,7 +35758,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="255" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B255" s="16"/>
       <c r="C255" s="12">
         <v>1</v>
@@ -35711,7 +35800,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="256" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B256" s="16"/>
       <c r="C256" s="13">
         <v>0.18170138888888887</v>
@@ -35753,7 +35842,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="257" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B257" s="17"/>
       <c r="C257" s="14">
         <v>0.18690972222222221</v>
@@ -35795,7 +35884,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="258" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B258" s="15" t="s">
         <v>140</v>
       </c>
@@ -35839,7 +35928,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="259" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B259" s="16"/>
       <c r="C259" s="12">
         <v>1</v>
@@ -35881,7 +35970,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="260" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B260" s="16"/>
       <c r="C260" s="13">
         <v>4.5127314814814821E-2</v>
@@ -35923,7 +36012,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="261" spans="2:15" ht="18" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
       <c r="B261" s="16"/>
       <c r="C261" s="13">
         <v>3.471064814814815E-2</v>
@@ -35965,7 +36054,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="262" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B262" s="16"/>
       <c r="C262" s="12">
         <v>-1733.3330000000001</v>
@@ -36007,7 +36096,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="263" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B263" s="16"/>
       <c r="C263" s="12">
         <v>1</v>
@@ -36049,7 +36138,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="264" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B264" s="16"/>
       <c r="C264" s="13">
         <v>0.10820601851851852</v>
@@ -36091,7 +36180,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="265" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B265" s="16"/>
       <c r="C265" s="13">
         <v>9.2581018518518521E-2</v>
@@ -36133,7 +36222,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B266" s="16"/>
       <c r="C266" s="12">
         <v>-1266.6669999999999</v>
@@ -36175,7 +36264,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="267" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B267" s="16"/>
       <c r="C267" s="12">
         <v>1</v>
@@ -36217,7 +36306,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="268" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B268" s="16"/>
       <c r="C268" s="13">
         <v>6.7118055555555556E-2</v>
@@ -36259,7 +36348,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="269" spans="2:15" ht="27" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
       <c r="B269" s="17"/>
       <c r="C269" s="14">
         <v>6.519675925925926E-2</v>
@@ -36317,4 +36406,65 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D391230B-B3E3-40C8-A871-F0677929209D}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="18" t="s">
+        <v>268</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>269</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>270</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>271</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>275</v>
+      </c>
+      <c r="B2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D2">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>278</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change the way equipment is stored to a dict
</commit_message>
<xml_diff>
--- a/cytation_H1_plate1.xlsx
+++ b/cytation_H1_plate1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\School Stuff\Sem 7\FYP\EBase + PBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D25F620-D0D5-4A25-AE54-FE04AC23DCA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B696303-617A-4FCB-B7D0-65958794C62B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="279">
   <si>
     <t>Software Version</t>
   </si>
@@ -845,9 +845,6 @@
     <t>Media</t>
   </si>
   <si>
-    <t>Equipment</t>
-  </si>
-  <si>
     <t>Plasmid name</t>
   </si>
   <si>
@@ -1388,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:CU269"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="L72" sqref="L72"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="M69" sqref="M69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -36410,15 +36407,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D391230B-B3E3-40C8-A871-F0677929209D}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>268</v>
       </c>
@@ -36437,31 +36434,25 @@
       <c r="F1" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="G1" s="18" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>275</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>276</v>
-      </c>
-      <c r="C2" t="s">
-        <v>277</v>
       </c>
       <c r="D2">
         <v>37</v>
       </c>
       <c r="E2" t="s">
+        <v>277</v>
+      </c>
+      <c r="F2" t="s">
         <v>278</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>279</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change how data values are stored to dict
</commit_message>
<xml_diff>
--- a/cytation_H1_plate1.xlsx
+++ b/cytation_H1_plate1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\School Stuff\Sem 7\FYP\EBase + PBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B696303-617A-4FCB-B7D0-65958794C62B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C08F7B-E7F1-4BCF-9B16-E23143E11BCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:CU269"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="M69" sqref="M69"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -36409,8 +36409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D391230B-B3E3-40C8-A871-F0677929209D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>